<commit_message>
Motivation: formatiert, Medienstreams, Stand-By; neues Eva-Bild
</commit_message>
<xml_diff>
--- a/Evaluationsergebnisse/Teilnehmerauswertung_Evaluation_Verteilte_Vorlesung_2.xlsx
+++ b/Evaluationsergebnisse/Teilnehmerauswertung_Evaluation_Verteilte_Vorlesung_2.xlsx
@@ -785,37 +785,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -831,11 +831,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="93858432"/>
-        <c:axId val="93872512"/>
+        <c:axId val="95955584"/>
+        <c:axId val="95969664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="93858432"/>
+        <c:axId val="95955584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -855,7 +855,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93872512"/>
+        <c:crossAx val="95969664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -863,9 +863,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93872512"/>
+        <c:axId val="95969664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="18"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -884,7 +885,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93858432"/>
+        <c:crossAx val="95955584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -895,10 +896,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.77777058093470863"/>
-          <c:y val="0.36313288993679421"/>
-          <c:w val="0.22222941906529142"/>
-          <c:h val="0.12239700399155504"/>
+          <c:x val="0.81788859811542003"/>
+          <c:y val="0.32236231628387346"/>
+          <c:w val="0.18211140188458"/>
+          <c:h val="0.1631675593803113"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -912,7 +913,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1000">
+        <a:defRPr sz="1050">
           <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
           <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
         </a:defRPr>
@@ -933,15 +934,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>247653</xdr:colOff>
+      <xdr:colOff>247654</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>157160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4229100</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>119061</xdr:rowOff>
+      <xdr:colOff>3993173</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>58615</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -962,16 +963,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2782358</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>11642</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>10583</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>106160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>4668308</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>2117</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>378394</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>96635</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -980,8 +981,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3544358" y="5345642"/>
-          <a:ext cx="1885950" cy="1133475"/>
+          <a:off x="11840633" y="3725660"/>
+          <a:ext cx="1891811" cy="1133475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1190,16 +1191,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2653852</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>180242</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>463105</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>117232</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3534833</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>183894</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>585017</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>120884</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1216,8 +1217,198 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="16200000">
-          <a:off x="3040923" y="6079671"/>
-          <a:ext cx="1630840" cy="880981"/>
+          <a:off x="11918897" y="5825490"/>
+          <a:ext cx="1632427" cy="883912"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>400212</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>95290</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11068050" y="7156450"/>
+          <a:ext cx="1162212" cy="285790"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>412750</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>184437</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>92108</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Grafik 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12242800" y="7200900"/>
+          <a:ext cx="2057687" cy="238158"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>606772</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>114340</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Grafik 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14478000" y="7175500"/>
+          <a:ext cx="2486372" cy="285790"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>133563</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>6385</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Grafik 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11201400" y="8058150"/>
+          <a:ext cx="1524213" cy="247685"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>403423</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>95285</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Grafik 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11576050" y="8337550"/>
+          <a:ext cx="1419423" cy="247685"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1521,8 +1712,8 @@
   </sheetPr>
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1588,11 +1779,11 @@
         <v>0</v>
       </c>
       <c r="G3" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H13" si="0">SUM(C3:G3)</f>
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1613,11 +1804,11 @@
         <v>0</v>
       </c>
       <c r="G4" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1638,11 +1829,11 @@
         <v>0</v>
       </c>
       <c r="G5" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1663,11 +1854,11 @@
         <v>0</v>
       </c>
       <c r="G6" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1690,11 +1881,11 @@
         <v>0</v>
       </c>
       <c r="G7" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1715,11 +1906,11 @@
         <v>1</v>
       </c>
       <c r="G8" s="6">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1740,11 +1931,11 @@
         <v>0</v>
       </c>
       <c r="G9" s="6">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1765,11 +1956,11 @@
         <v>2</v>
       </c>
       <c r="G10" s="6">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1792,11 +1983,11 @@
         <v>0</v>
       </c>
       <c r="G11" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1817,11 +2008,11 @@
         <v>0</v>
       </c>
       <c r="G12" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1842,11 +2033,11 @@
         <v>0</v>
       </c>
       <c r="G13" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="10:10" ht="23.45" x14ac:dyDescent="0.45">

</xml_diff>